<commit_message>
added two functions iRCT.py to show old methods
</commit_message>
<xml_diff>
--- a/docs/Info on causal learning algorithms.xlsx
+++ b/docs/Info on causal learning algorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17172\Desktop\iRCT\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0994B24D-F292-43D7-8BEA-FA5738E7A897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2088D9B2-1BD8-4D52-B081-546AD4332782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2925" windowWidth="15375" windowHeight="7875" xr2:uid="{C79AF796-9487-4DE7-B670-D48F198EEEE9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C79AF796-9487-4DE7-B670-D48F198EEEE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Algorithm Used</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>FGS</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,10 +483,16 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>